<commit_message>
update Format file Excel
</commit_message>
<xml_diff>
--- a/add-products/Product.xlsx
+++ b/add-products/Product.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyPC\Desktop\DAVISY-PRO1014\add-products\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyPC\Desktop\DAVISY-PRO1041\add-products\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>khong co mota</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>SP01</t>
+  </si>
+  <si>
+    <t>SỐ LƯỢNG</t>
   </si>
 </sst>
 </file>
@@ -404,20 +407,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="4" width="15.75" customWidth="1"/>
-    <col min="7" max="7" width="18.125" customWidth="1"/>
+    <col min="2" max="5" width="15.75" customWidth="1"/>
+    <col min="8" max="8" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -431,16 +434,19 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -454,16 +460,19 @@
         <v>3</v>
       </c>
       <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>300000</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>500000</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -477,16 +486,19 @@
         <v>4</v>
       </c>
       <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
         <v>400000</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>600000</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -500,16 +512,19 @@
         <v>3</v>
       </c>
       <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
         <v>300000</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>500000</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -523,12 +538,15 @@
         <v>3</v>
       </c>
       <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
         <v>300000</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>500000</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>